<commit_message>
Siap deploy ke Render
</commit_message>
<xml_diff>
--- a/hasil.xlsx
+++ b/hasil.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B236"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -412,15 +412,15 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>6281255290865</v>
+        <v>62811880123</v>
       </c>
       <c r="B2" t="str">
-        <v>Tidak Terdaftar WA</v>
+        <v>Terdaftar WA</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>6282175526975</v>
+        <v>5556285289846325</v>
       </c>
       <c r="B3" t="str">
         <v>Tidak Terdaftar WA</v>
@@ -428,31 +428,31 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>6281244860364</v>
+        <v>6281351844107</v>
       </c>
       <c r="B4" t="str">
-        <v>Terdaftar WA</v>
+        <v>Tidak Terdaftar WA</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>6281257887429</v>
+        <v>86628817798094</v>
       </c>
       <c r="B5" t="str">
-        <v>Terdaftar WA</v>
+        <v>Tidak Terdaftar WA</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>6285860507534</v>
+        <v>286285647739700</v>
       </c>
       <c r="B6" t="str">
-        <v>Terdaftar WA</v>
+        <v>Tidak Terdaftar WA</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>6288210806969</v>
+        <v>05056282278020755</v>
       </c>
       <c r="B7" t="str">
         <v>Tidak Terdaftar WA</v>
@@ -460,7 +460,7 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>6285733596155</v>
+        <v>1006281313873853</v>
       </c>
       <c r="B8" t="str">
         <v>Tidak Terdaftar WA</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>6282283332862</v>
+        <v>6282261559840</v>
       </c>
       <c r="B9" t="str">
         <v>Tidak Terdaftar WA</v>
@@ -476,31 +476,31 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>6283191524987</v>
+        <v>966285725803690</v>
       </c>
       <c r="B10" t="str">
-        <v>Terdaftar WA</v>
+        <v>Tidak Terdaftar WA</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>6281298811040</v>
+        <v>123456285724501595</v>
       </c>
       <c r="B11" t="str">
-        <v>Terdaftar WA</v>
+        <v>Tidak Terdaftar WA</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>6281349416712</v>
+        <v>12216285609715501</v>
       </c>
       <c r="B12" t="str">
-        <v>Terdaftar WA</v>
+        <v>Tidak Terdaftar WA</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>6282120066195</v>
+        <v>46282211333354</v>
       </c>
       <c r="B13" t="str">
         <v>Tidak Terdaftar WA</v>
@@ -508,15 +508,15 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>6285633259513</v>
+        <v>6289656591092</v>
       </c>
       <c r="B14" t="str">
-        <v>Tidak Terdaftar WA</v>
+        <v>Terdaftar WA</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>6285223208590</v>
+        <v>6281929756640</v>
       </c>
       <c r="B15" t="str">
         <v>Tidak Terdaftar WA</v>
@@ -524,7 +524,7 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>6285824593765</v>
+        <v>6285357066217</v>
       </c>
       <c r="B16" t="str">
         <v>Terdaftar WA</v>
@@ -532,7 +532,7 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>628128633987</v>
+        <v>123456285722742085</v>
       </c>
       <c r="B17" t="str">
         <v>Tidak Terdaftar WA</v>
@@ -540,15 +540,15 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>6282230227281</v>
+        <v>1234628881081181</v>
       </c>
       <c r="B18" t="str">
-        <v>Terdaftar WA</v>
+        <v>Tidak Terdaftar WA</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>6282281639620</v>
+        <v>303628977078432</v>
       </c>
       <c r="B19" t="str">
         <v>Tidak Terdaftar WA</v>
@@ -556,7 +556,7 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>6282164503235</v>
+        <v>126281272700252</v>
       </c>
       <c r="B20" t="str">
         <v>Tidak Terdaftar WA</v>
@@ -564,31 +564,31 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>6281320262997</v>
+        <v>0226281294443486</v>
       </c>
       <c r="B21" t="str">
-        <v>Terdaftar WA</v>
+        <v>Tidak Terdaftar WA</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>6282359154473</v>
+        <v>1062882001966221</v>
       </c>
       <c r="B22" t="str">
-        <v>Terdaftar WA</v>
+        <v>Tidak Terdaftar WA</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>6289602931917</v>
+        <v>806285388758767</v>
       </c>
       <c r="B23" t="str">
-        <v>Terdaftar WA</v>
+        <v>Tidak Terdaftar WA</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>6281267257601</v>
+        <v>886285718267677</v>
       </c>
       <c r="B24" t="str">
         <v>Tidak Terdaftar WA</v>
@@ -596,7 +596,7 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>6285215124375</v>
+        <v>6281234567890</v>
       </c>
       <c r="B25" t="str">
         <v>Tidak Terdaftar WA</v>
@@ -604,15 +604,15 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>6288216473722</v>
+        <v>6282116965561</v>
       </c>
       <c r="B26" t="str">
-        <v>Tidak Terdaftar WA</v>
+        <v>Terdaftar WA</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>6285353221548</v>
+        <v>1236285881394588</v>
       </c>
       <c r="B27" t="str">
         <v>Tidak Terdaftar WA</v>
@@ -620,15 +620,15 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>6285298029903</v>
+        <v>986285750711974</v>
       </c>
       <c r="B28" t="str">
-        <v>Terdaftar WA</v>
+        <v>Tidak Terdaftar WA</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>6285876094512</v>
+        <v>62821158963789</v>
       </c>
       <c r="B29" t="str">
         <v>Tidak Terdaftar WA</v>
@@ -636,7 +636,7 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>6285783296390</v>
+        <v>996285817692926</v>
       </c>
       <c r="B30" t="str">
         <v>Tidak Terdaftar WA</v>
@@ -644,15 +644,1655 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>6281219247745</v>
+        <v>16282160527459</v>
       </c>
       <c r="B31" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>6282307081611</v>
+      </c>
+      <c r="B32" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>286282213178315</v>
+      </c>
+      <c r="B33" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>696285223582963</v>
+      </c>
+      <c r="B34" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>886281317477778</v>
+      </c>
+      <c r="B35" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>6282350998923</v>
+      </c>
+      <c r="B36" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>106282194747219</v>
+      </c>
+      <c r="B37" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>1236283155859880</v>
+      </c>
+      <c r="B38" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>446285315642215</v>
+      </c>
+      <c r="B39" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>1236281413243886</v>
+      </c>
+      <c r="B40" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>236282215005221</v>
+      </c>
+      <c r="B41" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>20036285273934200</v>
+      </c>
+      <c r="B42" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>1236282397194279</v>
+      </c>
+      <c r="B43" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>836281314493999</v>
+      </c>
+      <c r="B44" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>026283123534198</v>
+      </c>
+      <c r="B45" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>27628998916179</v>
+      </c>
+      <c r="B46" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>106287790057296</v>
+      </c>
+      <c r="B47" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>6285223654987</v>
+      </c>
+      <c r="B48" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>306285792120958</v>
+      </c>
+      <c r="B49" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>086282186487649</v>
+      </c>
+      <c r="B50" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>776285361936648</v>
+      </c>
+      <c r="B51" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>6281320073633</v>
+      </c>
+      <c r="B52" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>1256282260637007</v>
+      </c>
+      <c r="B53" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>2346285223214537</v>
+      </c>
+      <c r="B54" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>80628568270408</v>
+      </c>
+      <c r="B55" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>6282112781212</v>
+      </c>
+      <c r="B56" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>9996285752047390</v>
+      </c>
+      <c r="B57" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>6281254890178</v>
+      </c>
+      <c r="B58" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>123456282312648040</v>
+      </c>
+      <c r="B59" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>9962895615780484</v>
+      </c>
+      <c r="B60" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>62895611729975</v>
+      </c>
+      <c r="B61" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>6282298632103</v>
+      </c>
+      <c r="B62" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>996281233873220</v>
+      </c>
+      <c r="B63" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>6281212761687</v>
+      </c>
+      <c r="B64" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>226285293103114</v>
+      </c>
+      <c r="B65" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>19906281574940224</v>
+      </c>
+      <c r="B66" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>696282122154147</v>
+      </c>
+      <c r="B67" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>856281294991660</v>
+      </c>
+      <c r="B68" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>996281345602788</v>
+      </c>
+      <c r="B69" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>6281286926680</v>
+      </c>
+      <c r="B70" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>016281225697856</v>
+      </c>
+      <c r="B71" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>176282154925573</v>
+      </c>
+      <c r="B72" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>216288215347221</v>
+      </c>
+      <c r="B73" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>40662811676767</v>
+      </c>
+      <c r="B74" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>23628124913494</v>
+      </c>
+      <c r="B75" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>0816281383280552</v>
+      </c>
+      <c r="B76" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>101062852123696321</v>
+      </c>
+      <c r="B77" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>56282243533166</v>
+      </c>
+      <c r="B78" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>016282370796563</v>
+      </c>
+      <c r="B79" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>1236281210790566</v>
+      </c>
+      <c r="B80" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>7776281252859955</v>
+      </c>
+      <c r="B81" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>996282215010288</v>
+      </c>
+      <c r="B82" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>7762813277171137</v>
+      </c>
+      <c r="B83" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>706282184040565</v>
+      </c>
+      <c r="B84" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>1262877456365496</v>
+      </c>
+      <c r="B85" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>16283894354391</v>
+      </c>
+      <c r="B86" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>226287743061870</v>
+      </c>
+      <c r="B87" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>026281234010088</v>
+      </c>
+      <c r="B88" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>2126285741234196</v>
+      </c>
+      <c r="B89" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>796282380842579</v>
+      </c>
+      <c r="B90" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>106281322355605</v>
+      </c>
+      <c r="B91" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>036285296374125</v>
+      </c>
+      <c r="B92" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>2404036282261986612</v>
+      </c>
+      <c r="B93" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>6285769185352</v>
+      </c>
+      <c r="B94" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>3476281517171617</v>
+      </c>
+      <c r="B95" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>196281349657440</v>
+      </c>
+      <c r="B96" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>996283160281293</v>
+      </c>
+      <c r="B97" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>6281910018469</v>
+      </c>
+      <c r="B98" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>0101628218803669</v>
+      </c>
+      <c r="B99" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>806281513689941</v>
+      </c>
+      <c r="B100" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>0000628558685550</v>
+      </c>
+      <c r="B101" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <v>886285863383266</v>
+      </c>
+      <c r="B102" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <v>123546281379040781</v>
+      </c>
+      <c r="B103" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="str">
+        <v>6281273930602</v>
+      </c>
+      <c r="B104" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="str">
+        <v>6282318353477</v>
+      </c>
+      <c r="B105" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="str">
+        <v>306281256456398</v>
+      </c>
+      <c r="B106" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="str">
+        <v>126281386233803</v>
+      </c>
+      <c r="B107" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="str">
+        <v>19956285257251313</v>
+      </c>
+      <c r="B108" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="str">
+        <v>226282240448229</v>
+      </c>
+      <c r="B109" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="str">
+        <v>996281266469868</v>
+      </c>
+      <c r="B110" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <v>6281253554790</v>
+      </c>
+      <c r="B111" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="str">
+        <v>106285651367450</v>
+      </c>
+      <c r="B112" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="str">
+        <v>37376285777718738</v>
+      </c>
+      <c r="B113" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="str">
+        <v>866281227249830</v>
+      </c>
+      <c r="B114" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="str">
+        <v>916282358875959</v>
+      </c>
+      <c r="B115" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="str">
+        <v>007628526396011</v>
+      </c>
+      <c r="B116" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="str">
+        <v>276285866416273</v>
+      </c>
+      <c r="B117" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="str">
+        <v>62822899536499</v>
+      </c>
+      <c r="B118" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="str">
+        <v>6281348013814</v>
+      </c>
+      <c r="B119" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="str">
+        <v>03086282240705218</v>
+      </c>
+      <c r="B120" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="str">
+        <v>016282111151512</v>
+      </c>
+      <c r="B121" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="str">
+        <v>116285227456369</v>
+      </c>
+      <c r="B122" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="str">
+        <v>6281291967964</v>
+      </c>
+      <c r="B123" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="str">
+        <v>6282299442893</v>
+      </c>
+      <c r="B124" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="str">
+        <v>6289681568188</v>
+      </c>
+      <c r="B125" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="str">
+        <v>6285322664977</v>
+      </c>
+      <c r="B126" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="str">
+        <v>946285591906027</v>
+      </c>
+      <c r="B127" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="str">
+        <v>6285934825870</v>
+      </c>
+      <c r="B128" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="str">
+        <v>1236285867453211</v>
+      </c>
+      <c r="B129" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="str">
+        <v>116287780496713</v>
+      </c>
+      <c r="B130" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="str">
+        <v>6287813006735</v>
+      </c>
+      <c r="B131" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="str">
+        <v>6281254898882</v>
+      </c>
+      <c r="B132" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="str">
+        <v>6287722293708</v>
+      </c>
+      <c r="B133" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="str">
+        <v>1236281234043716</v>
+      </c>
+      <c r="B134" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="str">
+        <v>20236285860331647</v>
+      </c>
+      <c r="B135" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="str">
+        <v>6281808243290</v>
+      </c>
+      <c r="B136" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="str">
+        <v>106282215181402</v>
+      </c>
+      <c r="B137" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="str">
+        <v>6287711166862</v>
+      </c>
+      <c r="B138" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="str">
+        <v>996287821961775</v>
+      </c>
+      <c r="B139" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="str">
+        <v>996285320993256</v>
+      </c>
+      <c r="B140" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="str">
+        <v>216283857713311</v>
+      </c>
+      <c r="B141" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="str">
+        <v>19876281220333551</v>
+      </c>
+      <c r="B142" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="str">
+        <v>6283822822917</v>
+      </c>
+      <c r="B143" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="str">
+        <v>6662895344056304</v>
+      </c>
+      <c r="B144" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="str">
+        <v>6285718123221</v>
+      </c>
+      <c r="B145" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="str">
+        <v>17526281330752875</v>
+      </c>
+      <c r="B146" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="str">
+        <v>6281219000502</v>
+      </c>
+      <c r="B147" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="str">
+        <v>016281379136857</v>
+      </c>
+      <c r="B148" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="str">
+        <v>106287790067290</v>
+      </c>
+      <c r="B149" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="str">
+        <v>6287777731382</v>
+      </c>
+      <c r="B150" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="str">
+        <v>8996281211825997</v>
+      </c>
+      <c r="B151" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="str">
+        <v>6287758491371</v>
+      </c>
+      <c r="B152" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="str">
+        <v>6282251569855</v>
+      </c>
+      <c r="B153" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="str">
+        <v>628999004463</v>
+      </c>
+      <c r="B154" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="str">
+        <v>6281542311356</v>
+      </c>
+      <c r="B155" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="str">
+        <v>6281313085519</v>
+      </c>
+      <c r="B156" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="str">
+        <v>116285334759859</v>
+      </c>
+      <c r="B157" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="str">
+        <v>800862811676767</v>
+      </c>
+      <c r="B158" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="str">
+        <v>086285890191919</v>
+      </c>
+      <c r="B159" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="str">
+        <v>6282134404384</v>
+      </c>
+      <c r="B160" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="str">
+        <v>116287739425384</v>
+      </c>
+      <c r="B161" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="str">
+        <v>00762812526655</v>
+      </c>
+      <c r="B162" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="str">
+        <v>116289632580</v>
+      </c>
+      <c r="B163" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="str">
+        <v>123456281389630257</v>
+      </c>
+      <c r="B164" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="str">
+        <v>6285624248471</v>
+      </c>
+      <c r="B165" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="str">
+        <v>1826289619837224</v>
+      </c>
+      <c r="B166" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="str">
+        <v>826285798023860</v>
+      </c>
+      <c r="B167" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="str">
+        <v>6281323158775</v>
+      </c>
+      <c r="B168" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="str">
+        <v>976285697420575</v>
+      </c>
+      <c r="B169" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="str">
+        <v>066281255627327</v>
+      </c>
+      <c r="B170" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="str">
+        <v>776281354978464</v>
+      </c>
+      <c r="B171" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="str">
+        <v>1236281375027287</v>
+      </c>
+      <c r="B172" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="str">
+        <v>1886281378523778</v>
+      </c>
+      <c r="B173" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="str">
+        <v>886281382355944</v>
+      </c>
+      <c r="B174" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="str">
+        <v>6285388399161</v>
+      </c>
+      <c r="B175" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="str">
+        <v>856285282998299</v>
+      </c>
+      <c r="B176" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="str">
+        <v>62813277175171</v>
+      </c>
+      <c r="B177" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="str">
+        <v>006281395686412</v>
+      </c>
+      <c r="B178" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="str">
+        <v>776281231105807</v>
+      </c>
+      <c r="B179" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="str">
+        <v>036287870416260</v>
+      </c>
+      <c r="B180" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="str">
+        <v>996282134550002</v>
+      </c>
+      <c r="B181" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="str">
+        <v>16285712696939</v>
+      </c>
+      <c r="B182" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="str">
+        <v>776281315649799</v>
+      </c>
+      <c r="B183" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="str">
+        <v>6281279614216</v>
+      </c>
+      <c r="B184" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="str">
+        <v>776281221404444</v>
+      </c>
+      <c r="B185" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="str">
+        <v>37786281378523778</v>
+      </c>
+      <c r="B186" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="str">
+        <v>1606281774960389</v>
+      </c>
+      <c r="B187" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="str">
+        <v>776285780581680</v>
+      </c>
+      <c r="B188" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="str">
+        <v>1156282117891033</v>
+      </c>
+      <c r="B189" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="str">
+        <v>86285845547594</v>
+      </c>
+      <c r="B190" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="str">
+        <v>196283895184874</v>
+      </c>
+      <c r="B191" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="str">
+        <v>116287875233698</v>
+      </c>
+      <c r="B192" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="str">
+        <v>206285793032491</v>
+      </c>
+      <c r="B193" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="str">
+        <v>3786282335311378</v>
+      </c>
+      <c r="B194" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="str">
+        <v>46285294393917</v>
+      </c>
+      <c r="B195" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="str">
+        <v>628175414622</v>
+      </c>
+      <c r="B196" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="str">
+        <v>196282141402033</v>
+      </c>
+      <c r="B197" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="str">
+        <v>1236281388687966</v>
+      </c>
+      <c r="B198" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="str">
+        <v>886287820222981</v>
+      </c>
+      <c r="B199" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="str">
+        <v>126281239545984</v>
+      </c>
+      <c r="B200" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="str">
+        <v>3336282217348779</v>
+      </c>
+      <c r="B201" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="str">
+        <v>226282179939401</v>
+      </c>
+      <c r="B202" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="str">
+        <v>6281252859944</v>
+      </c>
+      <c r="B203" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="str">
+        <v>2126285281768343</v>
+      </c>
+      <c r="B204" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="str">
+        <v>236285717325610</v>
+      </c>
+      <c r="B205" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="str">
+        <v>6281252859955</v>
+      </c>
+      <c r="B206" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="str">
+        <v>0266285221541231</v>
+      </c>
+      <c r="B207" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="str">
+        <v>906281215141996</v>
+      </c>
+      <c r="B208" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="str">
+        <v>90906281990690742</v>
+      </c>
+      <c r="B209" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="str">
+        <v>6282228000526</v>
+      </c>
+      <c r="B210" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="str">
+        <v>886285157200083</v>
+      </c>
+      <c r="B211" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="str">
+        <v>4206282299992421</v>
+      </c>
+      <c r="B212" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="str">
+        <v>976281289197839</v>
+      </c>
+      <c r="B213" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="str">
+        <v>896285746033493</v>
+      </c>
+      <c r="B214" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="str">
+        <v>126281290655146</v>
+      </c>
+      <c r="B215" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="str">
+        <v>1236288214401115</v>
+      </c>
+      <c r="B216" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="str">
+        <v>6289655452984</v>
+      </c>
+      <c r="B217" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="str">
+        <v>1136283134880185</v>
+      </c>
+      <c r="B218" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="str">
+        <v>12236285802047885</v>
+      </c>
+      <c r="B219" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="str">
+        <v>976283832376980</v>
+      </c>
+      <c r="B220" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="str">
+        <v>216289697009010</v>
+      </c>
+      <c r="B221" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="str">
+        <v>116281293397636</v>
+      </c>
+      <c r="B222" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="str">
+        <v>886285643181015</v>
+      </c>
+      <c r="B223" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="str">
+        <v>027628995059641</v>
+      </c>
+      <c r="B224" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="str">
+        <v>156282324089632</v>
+      </c>
+      <c r="B225" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="str">
+        <v>1236289763632580</v>
+      </c>
+      <c r="B226" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="str">
+        <v>3010926283834484997</v>
+      </c>
+      <c r="B227" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="str">
+        <v>10628787578788</v>
+      </c>
+      <c r="B228" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="str">
+        <v>99996281255714131</v>
+      </c>
+      <c r="B229" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="str">
+        <v>016285776611373</v>
+      </c>
+      <c r="B230" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="str">
+        <v>726287878602667</v>
+      </c>
+      <c r="B231" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="str">
+        <v>976285367310833</v>
+      </c>
+      <c r="B232" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="str">
+        <v>6285310303229</v>
+      </c>
+      <c r="B233" t="str">
+        <v>Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="str">
+        <v>1216282126829318</v>
+      </c>
+      <c r="B234" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="str">
+        <v>1236281239362142</v>
+      </c>
+      <c r="B235" t="str">
+        <v>Tidak Terdaftar WA</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="str">
+        <v>976281230633659</v>
+      </c>
+      <c r="B236" t="str">
         <v>Tidak Terdaftar WA</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B31"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B236"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>